<commit_message>
reflect kyonmm san review for graph
</commit_message>
<xml_diff>
--- a/roi_graph.xlsx
+++ b/roi_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,24 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>単価未調整</t>
-    <rPh sb="0" eb="2">
-      <t>タンカ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>ミチョウセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>単価調整</t>
-    <rPh sb="0" eb="4">
-      <t>タンカチョウセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>スモークテスト自動化</t>
     <phoneticPr fontId="1"/>
@@ -47,6 +30,14 @@
   </si>
   <si>
     <t>GUIテスト自動化</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストは内製でエンジニアは同一単価</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>手動テストは外注で、自動テストを内製化、手動と自動でエンジニアは別単価</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -177,7 +168,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>単価未調整</c:v>
+                  <c:v>テストは内製でエンジニアは同一単価</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -229,7 +220,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>単価調整</c:v>
+                  <c:v>手動テストは外注で、自動テストを内製化、手動と自動でエンジニアは別単価</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -285,11 +276,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111672904"/>
-        <c:axId val="2111678264"/>
+        <c:axId val="2089990648"/>
+        <c:axId val="2089982296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111672904"/>
+        <c:axId val="2089990648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,7 +299,6 @@
                   <a:rPr lang="ja-JP" altLang="en-US"/>
                   <a:t>ｔ</a:t>
                 </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -319,7 +309,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111678264"/>
+        <c:crossAx val="2089982296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -327,7 +317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111678264"/>
+        <c:axId val="2089982296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,7 +348,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111672904"/>
+        <c:crossAx val="2089990648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -380,6 +370,266 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>GUI</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>テスト自動化における</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>ROI</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>テストは内製でエンジニアは同一単価</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.873</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.548</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>手動テストは外注で、自動テストを内製化、手動と自動でエンジニアは別単価</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.472</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.878</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.317</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2091753496"/>
+        <c:axId val="2091759016"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2091753496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>t</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2091759016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2091759016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>ROI</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2091753496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -390,8 +640,8 @@
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>965200</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
@@ -407,6 +657,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="グラフ 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -740,19 +1020,19 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K21" sqref="K21:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -766,7 +1046,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1.0129999999999999</v>
@@ -777,7 +1057,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.50700000000000001</v>
@@ -791,13 +1071,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
       <c r="B10">
         <v>12</v>
       </c>
@@ -810,7 +1087,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>0.873</v>
@@ -821,7 +1098,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>0.47199999999999998</v>

</xml_diff>

<commit_message>
use oss at gui test on both case
</commit_message>
<xml_diff>
--- a/roi_graph.xlsx
+++ b/roi_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>スモークテスト自動化</t>
     <phoneticPr fontId="1"/>
@@ -30,6 +30,14 @@
   </si>
   <si>
     <t>GUIテスト自動化</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストは内製でエンジニアは同一単価</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>手動テストは外注で、自動テストを内製化、手動と自動でエンジニアは別単価</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -460,10 +468,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.873</c:v>
+                  <c:v>0.897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.548</c:v>
+                  <c:v>1.627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,7 +1028,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21:L21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1046,7 +1054,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1.0129999999999999</v>
@@ -1090,15 +1098,15 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <v>0.873</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="C11">
-        <v>1.548</v>
+        <v>1.627</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>0.47199999999999998</v>

</xml_diff>

<commit_message>
add descript roi function
</commit_message>
<xml_diff>
--- a/roi_graph.xlsx
+++ b/roi_graph.xlsx
@@ -33,7 +33,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>テストは内製でエンジニアは同一単価</t>
+    <t>手動テストは外注で、自動テストを内製化、手動と自動でエンジニアは別単価</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -45,7 +45,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>手動テストは外注で、自動テストを内製化、手動と自動でエンジニアは別単価</t>
+    <t>テストは内製でエンジニアは同一単価</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -284,11 +284,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2089990648"/>
-        <c:axId val="2089982296"/>
+        <c:axId val="2083986728"/>
+        <c:axId val="2083221320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2089990648"/>
+        <c:axId val="2083986728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -317,7 +317,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089982296"/>
+        <c:crossAx val="2083221320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -325,7 +325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089982296"/>
+        <c:axId val="2083221320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +356,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089990648"/>
+        <c:crossAx val="2083986728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -543,11 +543,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091753496"/>
-        <c:axId val="2091759016"/>
+        <c:axId val="2083265384"/>
+        <c:axId val="2083270904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091753496"/>
+        <c:axId val="2083265384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +577,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091759016"/>
+        <c:crossAx val="2083270904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -585,7 +585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091759016"/>
+        <c:axId val="2083270904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091753496"/>
+        <c:crossAx val="2083265384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1.0129999999999999</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0.50700000000000001</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>0.89700000000000002</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>0.47199999999999998</v>

</xml_diff>